<commit_message>
Fixed wellID indexing issue
</commit_message>
<xml_diff>
--- a/experiments/masterExperimentSpreadsheet.xlsx
+++ b/experiments/masterExperimentSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acharsr/Documents/Multiplexed-Flow-Data-Processing/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0D491A-5095-FE44-BA2E-C23E345549E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54637103-BD4E-8D45-B5DB-5DEA63AE28C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{FCB7D3D2-0F4C-8644-B223-566C67ECD71C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="55160" windowHeight="26720" xr2:uid="{FCB7D3D2-0F4C-8644-B223-566C67ECD71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -846,7 +846,7 @@
   <dimension ref="A1:U98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished single stains histogram module
</commit_message>
<xml_diff>
--- a/experiments/masterExperimentSpreadsheet.xlsx
+++ b/experiments/masterExperimentSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acharsr/Documents/Multiplexed-Flow-Data-Processing/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54637103-BD4E-8D45-B5DB-5DEA63AE28C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB7FEF0-A34B-7D4E-95F5-6DA60EE6AD5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="55160" windowHeight="26720" xr2:uid="{FCB7D3D2-0F4C-8644-B223-566C67ECD71C}"/>
+    <workbookView xWindow="14920" yWindow="2020" windowWidth="33600" windowHeight="18940" xr2:uid="{FCB7D3D2-0F4C-8644-B223-566C67ECD71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F26360F-6904-3846-B2C4-E5183148A5E9}">
   <dimension ref="A1:U98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished heatmaps,cbacorrections,emanuel robot data processing
</commit_message>
<xml_diff>
--- a/experiments/masterExperimentSpreadsheet.xlsx
+++ b/experiments/masterExperimentSpreadsheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acharsr/Documents/Multiplexed-Flow-Data-Processing/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB7FEF0-A34B-7D4E-95F5-6DA60EE6AD5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF1EFB3-730C-7043-9673-9C6179B18791}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="2020" windowWidth="33600" windowHeight="18940" xr2:uid="{FCB7D3D2-0F4C-8644-B223-566C67ECD71C}"/>
+    <workbookView xWindow="8800" yWindow="460" windowWidth="33600" windowHeight="19420" xr2:uid="{FCB7D3D2-0F4C-8644-B223-566C67ECD71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="160">
   <si>
     <t>Date</t>
   </si>
@@ -483,7 +484,34 @@
     <t>B16</t>
   </si>
   <si>
-    <t>last three timepoint supernantants dried out due to low incubator humidity</t>
+    <t>B16OVAIFNgPulsedKineticsPart1</t>
+  </si>
+  <si>
+    <t>B16OVAIFNgPulsedKineticsPart2</t>
+  </si>
+  <si>
+    <t>B16OVAIFNgPulsedKineticsPart3</t>
+  </si>
+  <si>
+    <t>last three timepoint supernantants dried out due to low incubator humidity, calibration's undiluted sample was weird for some reason; ended up discarding the sample for 15 total calibration solutions</t>
+  </si>
+  <si>
+    <t>322and412_CBA_Dilutions</t>
+  </si>
+  <si>
+    <t>DilutionCorrection</t>
+  </si>
+  <si>
+    <t>B16OVAIFNgPulsedConfluency</t>
+  </si>
+  <si>
+    <t>20190423-B16OVAIFNgPulsedConfluency_B16_Timeseries_1</t>
+  </si>
+  <si>
+    <t>1:5 Dilution not enough for N4 1uM IL2; will have to redo</t>
+  </si>
+  <si>
+    <t>404and308</t>
   </si>
 </sst>
 </file>
@@ -843,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F26360F-6904-3846-B2C4-E5183148A5E9}">
-  <dimension ref="A1:U98"/>
+  <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4275,7 +4303,7 @@
         <v>9</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" ref="G68:G98" si="5">B68&amp;"-"&amp;C68&amp;"_"&amp;D68&amp;"_"&amp;E68&amp;"_"&amp;F68</f>
+        <f t="shared" ref="G68:G104" si="5">B68&amp;"-"&amp;C68&amp;"_"&amp;D68&amp;"_"&amp;E68&amp;"_"&amp;F68</f>
         <v>20181018-PeptideComparison_OT1_Timeseries_9</v>
       </c>
       <c r="H68" t="s">
@@ -5380,7 +5408,7 @@
         <v>44</v>
       </c>
       <c r="I92" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="J92">
         <v>24</v>
@@ -5427,6 +5455,9 @@
       <c r="H93" t="s">
         <v>44</v>
       </c>
+      <c r="I93" t="s">
+        <v>75</v>
+      </c>
       <c r="J93">
         <v>24</v>
       </c>
@@ -5467,7 +5498,7 @@
         <v>44</v>
       </c>
       <c r="I94" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="J94">
         <v>16</v>
@@ -5592,17 +5623,26 @@
       <c r="H97" t="s">
         <v>44</v>
       </c>
+      <c r="I97" t="s">
+        <v>74</v>
+      </c>
       <c r="J97">
         <v>36</v>
       </c>
       <c r="K97">
         <v>16</v>
       </c>
+      <c r="L97">
+        <v>15</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
       <c r="Q97" t="s">
         <v>14</v>
       </c>
       <c r="R97" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
@@ -5644,7 +5684,256 @@
         <v>16</v>
       </c>
     </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>20190416</v>
+      </c>
+      <c r="C99" t="s">
+        <v>150</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E99" t="s">
+        <v>52</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="5"/>
+        <v>20190416-B16OVAIFNgPulsedKineticsPart1_B16_Timeseries_1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>141</v>
+      </c>
+      <c r="I99" t="s">
+        <v>75</v>
+      </c>
+      <c r="J99">
+        <v>3</v>
+      </c>
+      <c r="K99">
+        <v>8</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>20190416</v>
+      </c>
+      <c r="C100" t="s">
+        <v>151</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" t="s">
+        <v>52</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="5"/>
+        <v>20190416-B16OVAIFNgPulsedKineticsPart2_B16_Timeseries_1</v>
+      </c>
+      <c r="H100" t="s">
+        <v>141</v>
+      </c>
+      <c r="I100" t="s">
+        <v>75</v>
+      </c>
+      <c r="J100">
+        <v>3</v>
+      </c>
+      <c r="K100">
+        <v>48</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>20190416</v>
+      </c>
+      <c r="C101" t="s">
+        <v>152</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101" t="s">
+        <v>52</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="5"/>
+        <v>20190416-B16OVAIFNgPulsedKineticsPart3_B16_Timeseries_1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>141</v>
+      </c>
+      <c r="I101" t="s">
+        <v>75</v>
+      </c>
+      <c r="J101">
+        <v>5</v>
+      </c>
+      <c r="K101">
+        <v>48</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>20190423</v>
+      </c>
+      <c r="C102" t="s">
+        <v>156</v>
+      </c>
+      <c r="D102" t="s">
+        <v>149</v>
+      </c>
+      <c r="E102" t="s">
+        <v>52</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>157</v>
+      </c>
+      <c r="H102" t="s">
+        <v>141</v>
+      </c>
+      <c r="I102" t="s">
+        <v>75</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>96</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>20190426</v>
+      </c>
+      <c r="C103" t="s">
+        <v>154</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E103" t="s">
+        <v>155</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" si="5"/>
+        <v>20190426-322and412_CBA_Dilutions_OT1_DilutionCorrection_1</v>
+      </c>
+      <c r="H103" t="s">
+        <v>44</v>
+      </c>
+      <c r="I103" t="s">
+        <v>8</v>
+      </c>
+      <c r="J103">
+        <v>36</v>
+      </c>
+      <c r="K103">
+        <v>5</v>
+      </c>
+      <c r="L103">
+        <v>16</v>
+      </c>
+      <c r="M103">
+        <v>1</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>16</v>
+      </c>
+      <c r="R103" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>20190429</v>
+      </c>
+      <c r="C104" t="s">
+        <v>159</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E104" t="s">
+        <v>155</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" si="5"/>
+        <v>20190429-404and308_OT1_DilutionCorrection_2</v>
+      </c>
+      <c r="H104" t="s">
+        <v>44</v>
+      </c>
+      <c r="I104" t="s">
+        <v>8</v>
+      </c>
+      <c r="J104">
+        <v>36</v>
+      </c>
+      <c r="K104">
+        <v>16</v>
+      </c>
+      <c r="L104">
+        <v>16</v>
+      </c>
+      <c r="M104">
+        <v>1</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>